<commit_message>
modified immune signatures; added PBMC markers
</commit_message>
<xml_diff>
--- a/docs/tests/Ref/Immune_signatures.xlsx
+++ b/docs/tests/Ref/Immune_signatures.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cqian/Documents/GitHub/scMINER/tests/Ref/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lding/Git/scMINER/docs/tests/Ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFD31F8-504F-2945-83A4-B6440C70E5C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C85A4B-AC5C-7143-A60C-F8FCB74A7174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="2260" windowWidth="25020" windowHeight="25660" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="56220" yWindow="500" windowWidth="31640" windowHeight="28300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invitrogen_Cell_Marker_Mouse" sheetId="6" r:id="rId1"/>
     <sheet name="Markers_hg19" sheetId="5" r:id="rId2"/>
-    <sheet name="Cluster specific TF list2" sheetId="3" r:id="rId3"/>
-    <sheet name="Cluster specific TF list1" sheetId="1" r:id="rId4"/>
-    <sheet name="Makers_finer" sheetId="8" r:id="rId5"/>
+    <sheet name="Markers_hg19_Adam" sheetId="9" r:id="rId3"/>
+    <sheet name="Cluster specific TF list2" sheetId="3" r:id="rId4"/>
+    <sheet name="Cluster specific TF list1" sheetId="1" r:id="rId5"/>
+    <sheet name="Makers_finer" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="583">
   <si>
     <t>GN</t>
   </si>
@@ -1754,6 +1755,33 @@
   </si>
   <si>
     <t>CD20</t>
+  </si>
+  <si>
+    <t>CD4Mem</t>
+  </si>
+  <si>
+    <t>CD8Mem</t>
+  </si>
+  <si>
+    <t>CD8EffMem</t>
+  </si>
+  <si>
+    <t>Mono/DC</t>
+  </si>
+  <si>
+    <t>CCDC50</t>
+  </si>
+  <si>
+    <t>IRF7</t>
+  </si>
+  <si>
+    <t>Platelet</t>
+  </si>
+  <si>
+    <t>GNG11</t>
+  </si>
+  <si>
+    <t>PPBP</t>
   </si>
 </sst>
 </file>
@@ -1897,7 +1925,107 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2316,7 +2444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1E0FB8-404E-4849-BEA1-508F65B82C26}">
   <dimension ref="A1:B709"/>
   <sheetViews>
-    <sheetView topLeftCell="A257" workbookViewId="0">
+    <sheetView topLeftCell="A652" workbookViewId="0">
       <selection activeCell="B194" sqref="B194"/>
     </sheetView>
   </sheetViews>
@@ -8006,13 +8134,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BC333B-7BAA-384B-B8E1-81A7F388BD7A}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C45" sqref="A1:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -8513,22 +8642,610 @@
     <row r="62" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C74:C1048576 C35:C45 C17:C33 C1:C15">
-    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>-1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>-1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+      <formula>-1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC04E52-DC85-3842-B327-621E7A43442E}">
+  <dimension ref="A1:C48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>549</v>
+      </c>
+      <c r="C34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>557</v>
+      </c>
+      <c r="C35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B39" t="s">
+        <v>551</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B40" t="s">
+        <v>556</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B42" t="s">
+        <v>557</v>
+      </c>
+      <c r="C42">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B43" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="B45" t="s">
+        <v>578</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="B46" t="s">
+        <v>579</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="16" t="s">
+        <v>580</v>
+      </c>
+      <c r="B47" t="s">
+        <v>581</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
+        <v>580</v>
+      </c>
+      <c r="B48" t="s">
+        <v>582</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C17:C33 C1:C15 C35:C46">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>-1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>-1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>-1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>-1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>-1</formula>
     </cfRule>
@@ -8540,7 +9257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9650DA6-736B-D44E-BA08-149DB0EAC0AB}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -8837,7 +9554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -9471,11 +10188,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83782D9-153D-B04D-95A1-30FF008F9EC8}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>

</xml_diff>